<commit_message>
Updated a3_data in tabular folder; added sequence IDs, gene, and species
</commit_message>
<xml_diff>
--- a/tabular/a3_data.xlsx
+++ b/tabular/a3_data.xlsx
@@ -1,16 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/host/A3G-GLUE/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81023312-82AD-8C49-8043-D1EB2D683230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19420" yWindow="4420" windowWidth="18220" windowHeight="13100" tabRatio="500"/>
+    <workbookView xWindow="4780" yWindow="1840" windowWidth="24100" windowHeight="13100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
   <si>
     <t>NM_004900</t>
   </si>
@@ -85,13 +97,166 @@
   </si>
   <si>
     <t>SequenceID</t>
+  </si>
+  <si>
+    <t>APOBEC3B</t>
+  </si>
+  <si>
+    <t>APOBEC3G</t>
+  </si>
+  <si>
+    <t>NM_145298</t>
+  </si>
+  <si>
+    <t>APOBEC3Fv1</t>
+  </si>
+  <si>
+    <t>Gene</t>
+  </si>
+  <si>
+    <t>APOBEC3D</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Homo Sapiens</t>
+  </si>
+  <si>
+    <t>Pan troglodytes</t>
+  </si>
+  <si>
+    <t>NM_001349436</t>
+  </si>
+  <si>
+    <t>APOBEC3Gv2</t>
+  </si>
+  <si>
+    <t>APOBEC3C</t>
+  </si>
+  <si>
+    <t>XM_525658</t>
+  </si>
+  <si>
+    <t>APOBEC3FvX1</t>
+  </si>
+  <si>
+    <t>APOBEC3A</t>
+  </si>
+  <si>
+    <t>APOBEC3Av1</t>
+  </si>
+  <si>
+    <t>APOBEC3</t>
+  </si>
+  <si>
+    <t>Rattus norvegicus</t>
+  </si>
+  <si>
+    <t>Sus scrofa</t>
+  </si>
+  <si>
+    <t>APOBEC3H</t>
+  </si>
+  <si>
+    <t>Bos taurus</t>
+  </si>
+  <si>
+    <t>Equus caballus</t>
+  </si>
+  <si>
+    <t>Elephantulus edwardii</t>
+  </si>
+  <si>
+    <t>Lipotes vexillifer</t>
+  </si>
+  <si>
+    <t>APOBEC3AvX1</t>
+  </si>
+  <si>
+    <t>Oryctolagus cuniculus</t>
+  </si>
+  <si>
+    <t>Bison bison bison</t>
+  </si>
+  <si>
+    <t>APOBEC3HvX2</t>
+  </si>
+  <si>
+    <t>Odobenus rosmarus</t>
+  </si>
+  <si>
+    <t>XM_024452179</t>
+  </si>
+  <si>
+    <t>XM_017861318</t>
+  </si>
+  <si>
+    <t>XM_023515456</t>
+  </si>
+  <si>
+    <t>XM_021708335</t>
+  </si>
+  <si>
+    <t>XM_015457184</t>
+  </si>
+  <si>
+    <t>XM_011964203</t>
+  </si>
+  <si>
+    <t>XM_021676043</t>
+  </si>
+  <si>
+    <t>APOBEC3F-likexV1</t>
+  </si>
+  <si>
+    <t>Colobus angolensis palliatus</t>
+  </si>
+  <si>
+    <t>Macaca fascicularis</t>
+  </si>
+  <si>
+    <t>Rousettus aegyptiacus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manis javanica </t>
+  </si>
+  <si>
+    <t>APOBEC3FvX2</t>
+  </si>
+  <si>
+    <t>Rhinopithecus bieti</t>
+  </si>
+  <si>
+    <t>APOBEC3G-like</t>
+  </si>
+  <si>
+    <t>Aotus nancymaae</t>
+  </si>
+  <si>
+    <t>APOBEC3C-like</t>
+  </si>
+  <si>
+    <t>Carlito syrichta</t>
+  </si>
+  <si>
+    <t>Otolemur garnettii</t>
+  </si>
+  <si>
+    <t>Homo sapiens</t>
+  </si>
+  <si>
+    <t>Neophocaena asiaeorientalis</t>
+  </si>
+  <si>
+    <t>Bos indicus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,13 +265,27 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -121,14 +300,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -453,127 +641,376 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>20</v>
       </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C34">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>